<commit_message>
boton atras + refactor + herenciaToolbar
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 3ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 3ª Version.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FD4461-3B00-4266-AE52-E12D2872766D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD7A7B5-0ABB-440F-AFDA-61EF6AA048BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,7 +655,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,12 +776,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF34A853"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -891,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -963,7 +957,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1638,8 +1631,8 @@
   </sheetPr>
   <dimension ref="A2:P118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1693,38 +1686,38 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>246.18999999999994</v>
+        <v>249.85999999999993</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="50">
+      <c r="K3" s="49">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73</f>
-        <v>58.95</v>
+        <v>58.75</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="50"/>
+      <c r="K4" s="49"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="50"/>
+      <c r="K5" s="49"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -1744,10 +1737,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="52">
+      <c r="K6" s="51">
         <f>F7+F13+F20+F43+F45+F47+F46+J76</f>
         <v>31.5</v>
       </c>
@@ -1770,8 +1763,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="51"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -1791,8 +1784,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="51"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -1812,12 +1805,12 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="53" t="s">
+      <c r="J9" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="52">
+      <c r="K9" s="51">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74</f>
-        <v>64.59</v>
+        <v>68.260000000000005</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1837,8 +1830,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="51"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -1855,8 +1848,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="51"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -1875,10 +1868,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="52">
+      <c r="K12" s="51">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77</f>
         <v>36.6</v>
       </c>
@@ -1898,8 +1891,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="52"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="51"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -1916,8 +1909,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="52"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="51"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -1934,10 +1927,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="52">
+      <c r="K15" s="51">
         <f>F10+F16+F39+F40+F49+F50+F51+J75</f>
         <v>28</v>
       </c>
@@ -1957,8 +1950,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="52"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="51"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -1975,8 +1968,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="52"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="51"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -1995,10 +1988,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="56" t="s">
+      <c r="J18" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="52">
+      <c r="K18" s="51">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+F79+F82+F81+J78</f>
         <v>30.25</v>
       </c>
@@ -2021,8 +2014,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="52"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="51"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2041,8 +2034,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="52"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="51"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2079,11 +2072,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="57" t="s">
+      <c r="J22" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2405,22 +2398,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="49"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3092,14 +3085,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="49" t="s">
+      <c r="B72" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="49"/>
-      <c r="D72" s="49"/>
-      <c r="E72" s="49"/>
-      <c r="F72" s="49"/>
-      <c r="G72" s="49"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="48"/>
+      <c r="F72" s="48"/>
+      <c r="G72" s="48"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3111,18 +3104,18 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="49"/>
-      <c r="C73" s="49"/>
-      <c r="D73" s="49"/>
-      <c r="E73" s="49"/>
-      <c r="F73" s="49"/>
-      <c r="G73" s="49"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J73">
-        <f>F74+F83+F91+F93+F94+F95</f>
-        <v>9.75</v>
+        <f>F74+F83+F92+F93+F94+F95+F105+F106+F107+F108</f>
+        <v>9.5500000000000007</v>
       </c>
       <c r="K73">
         <f>E74+E83+E92+E93+E94+E95</f>
@@ -3150,8 +3143,8 @@
         <v>13</v>
       </c>
       <c r="J74">
-        <f>F80+F91+F102+F104+F103</f>
-        <v>18.869999999999997</v>
+        <f>F80+F91+F102+F104+F103+F115+F116+F117</f>
+        <v>22.54</v>
       </c>
       <c r="K74">
         <f>E80+E91</f>
@@ -3320,7 +3313,7 @@
       <c r="F82" s="34">
         <v>2</v>
       </c>
-      <c r="G82" s="34"/>
+      <c r="G82" s="11"/>
     </row>
     <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
@@ -3454,9 +3447,9 @@
       </c>
       <c r="E91" s="34"/>
       <c r="F91" s="34">
-        <v>3.7</v>
-      </c>
-      <c r="G91" s="34"/>
+        <v>4.2</v>
+      </c>
+      <c r="G91" s="11"/>
     </row>
     <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
@@ -3634,7 +3627,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="34">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G102" s="7"/>
     </row>
@@ -3652,7 +3645,7 @@
         <v>2</v>
       </c>
       <c r="F103" s="1">
-        <v>3.17</v>
+        <v>4.17</v>
       </c>
       <c r="G103" s="11"/>
     </row>
@@ -3857,8 +3850,10 @@
       <c r="E116" s="34">
         <v>7</v>
       </c>
-      <c r="F116" s="34"/>
-      <c r="G116" s="34"/>
+      <c r="F116" s="34">
+        <v>0.17</v>
+      </c>
+      <c r="G116" s="11"/>
     </row>
     <row r="117" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="45" t="s">
@@ -3872,15 +3867,15 @@
         <v>0.5</v>
       </c>
       <c r="F117" s="46">
-        <v>0</v>
-      </c>
-      <c r="G117" s="47"/>
+        <v>1.5</v>
+      </c>
+      <c r="G117" s="11"/>
     </row>
     <row r="118" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C118" s="48" t="s">
+      <c r="C118" s="47" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4878,14 +4873,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -5094,6 +5081,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
@@ -5103,23 +5098,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5136,4 +5114,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cartel carta más alta
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 3ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 3ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD7A7B5-0ABB-440F-AFDA-61EF6AA048BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C6D448-5CC7-419A-A102-F2A3178A012A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="170">
   <si>
     <t>Nombre</t>
   </si>
@@ -570,6 +570,12 @@
   </si>
   <si>
     <t>boton de volumen</t>
+  </si>
+  <si>
+    <t>Hacer cartel + frontal blackjack</t>
+  </si>
+  <si>
+    <t>TDD konguitorun</t>
   </si>
 </sst>
 </file>
@@ -655,7 +661,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +782,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -885,7 +897,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -985,6 +997,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,7 +1066,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>16770</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>13218</xdr:rowOff>
+      <xdr:rowOff>10043</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1114,7 +1127,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>15688</xdr:rowOff>
+      <xdr:rowOff>12513</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1175,7 +1188,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>16769</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>11785</xdr:rowOff>
+      <xdr:rowOff>8610</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1358,7 +1371,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>13261</xdr:rowOff>
+      <xdr:rowOff>10086</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1629,22 +1642,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P118"/>
+  <dimension ref="A2:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.21875" customWidth="1"/>
-    <col min="11" max="11" width="35.44140625" customWidth="1"/>
-    <col min="12" max="12" width="26.77734375" customWidth="1"/>
-    <col min="16" max="16" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.1796875" customWidth="1"/>
+    <col min="11" max="11" width="35.453125" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1673,7 +1686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1682,20 +1695,20 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E992)</f>
-        <v>226.2</v>
+        <v>232.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>249.85999999999993</v>
+        <v>251.35999999999993</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
       <c r="K3" s="49">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73</f>
-        <v>58.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>60.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="48" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +1722,7 @@
       </c>
       <c r="K4" s="49"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -2017,7 +2030,7 @@
       <c r="J19" s="55"/>
       <c r="K19" s="51"/>
     </row>
-    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2037,7 +2050,7 @@
       <c r="J20" s="55"/>
       <c r="K20" s="51"/>
     </row>
-    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2055,7 +2068,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2078,7 +2091,7 @@
       <c r="K22" s="56"/>
       <c r="L22" s="56"/>
     </row>
-    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2096,7 +2109,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2114,7 +2127,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2132,7 +2145,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2150,7 +2163,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2168,7 +2181,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2186,7 +2199,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2204,7 +2217,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2222,7 +2235,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2239,7 +2252,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2257,7 +2270,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2271,7 +2284,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2289,7 +2302,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2307,7 +2320,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2325,7 +2338,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2343,7 +2356,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2361,7 +2374,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2379,7 +2392,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2397,7 +2410,7 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B41" s="48" t="s">
         <v>36</v>
       </c>
@@ -2407,7 +2420,7 @@
       <c r="F41" s="48"/>
       <c r="G41" s="48"/>
     </row>
-    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B42" s="48"/>
       <c r="C42" s="48"/>
       <c r="D42" s="48"/>
@@ -2415,7 +2428,7 @@
       <c r="F42" s="48"/>
       <c r="G42" s="48"/>
     </row>
-    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -2433,7 +2446,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -2451,7 +2464,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -2469,7 +2482,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2487,7 +2500,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -2505,7 +2518,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -2523,7 +2536,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -2550,7 +2563,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -2579,7 +2592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -2608,7 +2621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -2637,7 +2650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -2666,7 +2679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -2695,7 +2708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -2722,7 +2735,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -2740,7 +2753,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -2758,7 +2771,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -2785,7 +2798,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -2814,7 +2827,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -2843,7 +2856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3114,8 +3127,8 @@
         <v>9</v>
       </c>
       <c r="J73">
-        <f>F74+F83+F92+F93+F94+F95+F105+F106+F107+F108</f>
-        <v>9.5500000000000007</v>
+        <f>F74+F83+F92+F93+F94+F95+F105+F106+F107+F108+F119+F120</f>
+        <v>11.05</v>
       </c>
       <c r="K73">
         <f>E74+E83+E92+E93+E94+E95</f>
@@ -3347,7 +3360,7 @@
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -3487,7 +3500,7 @@
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="2:7" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -3878,6 +3891,40 @@
       <c r="C118" s="47" t="s">
         <v>125</v>
       </c>
+    </row>
+    <row r="119" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="D119" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E119" s="34">
+        <v>2</v>
+      </c>
+      <c r="F119" s="34">
+        <v>1.5</v>
+      </c>
+      <c r="G119" s="7"/>
+    </row>
+    <row r="120" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D120" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E120" s="34">
+        <v>4</v>
+      </c>
+      <c r="F120" s="34"/>
+      <c r="G120" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -3914,13 +3961,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3983,7 +4030,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -4004,7 +4051,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -4242,7 +4289,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -4263,7 +4310,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -4284,7 +4331,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -4301,7 +4348,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -4322,7 +4369,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -4337,7 +4384,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -4352,7 +4399,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -4373,7 +4420,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -4388,7 +4435,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -4411,7 +4458,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -4426,7 +4473,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -4449,7 +4496,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -4464,7 +4511,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -4479,7 +4526,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -4502,7 +4549,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -4523,7 +4570,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -4544,7 +4591,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -4565,7 +4612,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -4580,7 +4627,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -4595,7 +4642,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -4618,7 +4665,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -4633,7 +4680,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -4648,7 +4695,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -4669,7 +4716,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -4692,7 +4739,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -4715,7 +4762,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -4738,7 +4785,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -4761,7 +4808,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -4782,7 +4829,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -4797,7 +4844,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -4864,12 +4911,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5082,17 +5128,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5117,18 +5173,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
temp hechos pero falta colocarlos
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 3ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 3ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F785CB92-20E9-44DD-858B-F3B27EA2B247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D1312C-81CC-457F-9633-503A479FADD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1064,9 +1064,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>16770</xdr:colOff>
+      <xdr:colOff>20580</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>10043</xdr:rowOff>
+      <xdr:rowOff>11948</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1127,7 +1127,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>12513</xdr:rowOff>
+      <xdr:rowOff>16323</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1186,9 +1186,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>16769</xdr:colOff>
+      <xdr:colOff>20579</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>8610</xdr:rowOff>
+      <xdr:rowOff>10515</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1247,9 +1247,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>16769</xdr:colOff>
+      <xdr:colOff>20579</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>19275</xdr:rowOff>
+      <xdr:rowOff>15465</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1371,7 +1371,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>10086</xdr:rowOff>
+      <xdr:rowOff>11991</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1644,8 +1644,8 @@
   </sheetPr>
   <dimension ref="A2:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>260.35999999999996</v>
+        <v>262.35999999999996</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="K9" s="52">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74</f>
-        <v>73.260000000000005</v>
+        <v>75.260000000000005</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -3131,8 +3131,8 @@
         <v>15.05</v>
       </c>
       <c r="K73">
-        <f>E74+E83+E92+E93+E94+E95</f>
-        <v>11</v>
+        <f>E74+E83+E92+E93+E94+E95+E105+E106+E107+E108+E119+E120</f>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="J74">
         <f>F80+F91+F102+F104+F103+F115+F116+F117</f>
-        <v>27.54</v>
+        <v>29.54</v>
       </c>
       <c r="K74">
         <f>E80+E91+E102+E103+E104+E115+E116+E117</f>
@@ -3294,7 +3294,7 @@
       <c r="F80" s="34">
         <v>8.5</v>
       </c>
-      <c r="G80" s="11"/>
+      <c r="G80" s="7"/>
     </row>
     <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
@@ -3852,7 +3852,7 @@
         <v>5</v>
       </c>
       <c r="F115" s="34">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G115" s="11"/>
     </row>
@@ -4917,6 +4917,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -5125,15 +5134,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5143,6 +5143,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5157,14 +5165,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
actualización Demo 3 excel
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 3ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 3ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B228EB-414B-4C80-B75A-E0283E79C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C158C4A-FDBD-4F37-9250-7ED1C97E3979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="174">
   <si>
     <t>Nombre</t>
   </si>
@@ -585,6 +585,9 @@
   </si>
   <si>
     <t>Investigar/Ver tutoriales sobre socket programming</t>
+  </si>
+  <si>
+    <t>Arrancar la aplicación por cmd en una máquina vacía (investiagación)</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -667,12 +670,6 @@
       <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1009,30 +1006,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1042,32 +1015,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2089,8 +2086,8 @@
   </sheetPr>
   <dimension ref="A2:P123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2140,15 +2137,15 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E995)</f>
-        <v>238.2</v>
+        <v>242.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>278.85999999999996</v>
+        <v>286.95999999999998</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="50">
+      <c r="K3" s="53">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73</f>
         <v>80.75</v>
       </c>
@@ -2157,25 +2154,25 @@
       <c r="B4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="50"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="50"/>
+      <c r="K5" s="53"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2195,12 +2192,12 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="52">
+      <c r="K6" s="57">
         <f>F7+F13+F20+F43+F45+F47+F46+J76</f>
-        <v>31.5</v>
+        <v>39.6</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -2221,8 +2218,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="52"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2242,8 +2239,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="52"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2263,10 +2260,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="53" t="s">
+      <c r="J9" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="52">
+      <c r="K9" s="57">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74</f>
         <v>75.260000000000005</v>
       </c>
@@ -2288,8 +2285,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="57"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2306,8 +2303,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="52"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2326,10 +2323,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="52">
+      <c r="K12" s="57">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77</f>
         <v>36.6</v>
       </c>
@@ -2349,8 +2346,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="52"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="57"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2367,8 +2364,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="52"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="57"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2385,10 +2382,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="52">
+      <c r="K15" s="57">
         <f>F10+F16+F39+F40+F49+F50+F51+J75</f>
         <v>28</v>
       </c>
@@ -2408,8 +2405,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="52"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="57"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2426,8 +2423,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="52"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="57"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2446,10 +2443,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="56" t="s">
+      <c r="J18" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="52">
+      <c r="K18" s="57">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+F79+F82+F81+J78</f>
         <v>30.25</v>
       </c>
@@ -2472,8 +2469,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="52"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="57"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2492,8 +2489,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="52"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="57"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2530,11 +2527,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="57" t="s">
+      <c r="J22" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2859,19 +2856,19 @@
       <c r="B41" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="59"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3546,11 +3543,11 @@
       <c r="B72" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
+      <c r="C72" s="50"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="50"/>
+      <c r="G72" s="50"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3562,12 +3559,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="59"/>
-      <c r="C73" s="60"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="60"/>
-      <c r="F73" s="60"/>
-      <c r="G73" s="60"/>
+      <c r="B73" s="51"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="F73" s="52"/>
+      <c r="G73" s="52"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -3619,9 +3616,13 @@
       <c r="D75" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="34"/>
+      <c r="E75" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F75" s="34">
+        <v>2</v>
+      </c>
+      <c r="G75" s="7"/>
       <c r="I75" s="9" t="s">
         <v>15</v>
       </c>
@@ -3652,11 +3653,11 @@
       </c>
       <c r="J76">
         <f>F75+F89+F90+F99+F100</f>
-        <v>0</v>
+        <v>8.1</v>
       </c>
       <c r="K76">
         <f>E75+E89+E90+E99+E100</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3874,8 +3875,10 @@
       <c r="E89" s="34">
         <v>1</v>
       </c>
-      <c r="F89" s="34"/>
-      <c r="G89" s="34"/>
+      <c r="F89" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="G89" s="7"/>
     </row>
     <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
@@ -3890,8 +3893,10 @@
       <c r="E90" s="34">
         <v>2</v>
       </c>
-      <c r="F90" s="34"/>
-      <c r="G90" s="34"/>
+      <c r="F90" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="G90" s="7"/>
     </row>
     <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
@@ -4038,13 +4043,17 @@
         <v>12</v>
       </c>
       <c r="C99" s="37" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="D99" s="37">
         <v>48</v>
       </c>
-      <c r="E99" s="37"/>
-      <c r="F99" s="37"/>
+      <c r="E99" s="37">
+        <v>3</v>
+      </c>
+      <c r="F99" s="37">
+        <v>5</v>
+      </c>
       <c r="G99" s="11"/>
     </row>
     <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4055,9 +4064,13 @@
         <v>145</v>
       </c>
       <c r="D100" s="34"/>
-      <c r="E100" s="34"/>
-      <c r="F100" s="34"/>
-      <c r="G100" s="34"/>
+      <c r="E100" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="F100" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="G100" s="7"/>
     </row>
     <row r="101" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="40" t="s">
@@ -5418,11 +5431,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5635,27 +5649,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5680,9 +5684,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excel y cambio de alerta Tragaperras
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 3ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 3ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C158C4A-FDBD-4F37-9250-7ED1C97E3979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9A4BC4-F399-48F8-BCAA-BE7A12297B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2086,8 +2086,8 @@
   </sheetPr>
   <dimension ref="A2:P123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K81" sqref="K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>286.95999999999998</v>
+        <v>292.95999999999998</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="K6" s="57">
         <f>F7+F13+F20+F43+F45+F47+F46+J76</f>
-        <v>39.6</v>
+        <v>45.6</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -3652,12 +3652,12 @@
         <v>12</v>
       </c>
       <c r="J76">
-        <f>F75+F89+F90+F99+F100</f>
-        <v>8.1</v>
+        <f>F75+F89+F90+F99+F100+F115+F116+F117</f>
+        <v>14.1</v>
       </c>
       <c r="K76">
-        <f>E75+E89+E90+E99+E100</f>
-        <v>7</v>
+        <f>E75+E89+E90+E99+E100+E115+E116+E117</f>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4321,8 +4321,10 @@
       <c r="E115" s="37">
         <v>10</v>
       </c>
-      <c r="F115" s="37"/>
-      <c r="G115" s="37"/>
+      <c r="F115" s="37">
+        <v>6</v>
+      </c>
+      <c r="G115" s="11"/>
     </row>
     <row r="116" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
@@ -5431,12 +5433,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5649,17 +5650,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5684,18 +5695,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Soporte al cliente en plantilla
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 3ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 3ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9A4BC4-F399-48F8-BCAA-BE7A12297B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D998292-048C-4D89-BD0F-F37B9A8EF5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2086,8 +2086,8 @@
   </sheetPr>
   <dimension ref="A2:P123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K81" sqref="K81"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2196,8 +2196,8 @@
         <v>12</v>
       </c>
       <c r="K6" s="57">
-        <f>F7+F13+F20+F43+F45+F47+F46+J76</f>
-        <v>45.6</v>
+        <f>F7+F13+F20+F43+F45+F47+F46+J76+F75+F89+F90+F99+F100+F115+F116+F117</f>
+        <v>59.7</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -5433,11 +5433,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5650,27 +5651,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5695,9 +5686,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
musica perfil y eventos
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 3ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 3ª Version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B228EB-414B-4C80-B75A-E0283E79C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE26C9A-0C8F-4DCC-B8D0-A3E526341C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -569,9 +569,6 @@
     <t xml:space="preserve">idiomas </t>
   </si>
   <si>
-    <t>boton de volumen</t>
-  </si>
-  <si>
     <t>Hacer cartel + frontal blackjack</t>
   </si>
   <si>
@@ -585,6 +582,9 @@
   </si>
   <si>
     <t>Investigar/Ver tutoriales sobre socket programming</t>
+  </si>
+  <si>
+    <t>boton de volumen (mutear)</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -667,12 +667,6 @@
       <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1009,30 +1003,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1042,32 +1012,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1137,7 +1131,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>20580</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>11948</xdr:rowOff>
+      <xdr:rowOff>19568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1259,7 +1253,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>20579</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>10515</xdr:rowOff>
+      <xdr:rowOff>16230</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1380,8 +1374,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>3025</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>193504</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3004</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1442,7 +1436,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>11991</xdr:rowOff>
+      <xdr:rowOff>19611</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2089,8 +2083,8 @@
   </sheetPr>
   <dimension ref="A2:P123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2140,15 +2134,15 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E995)</f>
-        <v>238.2</v>
+        <v>238.7</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>278.85999999999996</v>
+        <v>282.86999999999995</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="50">
+      <c r="K3" s="53">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73</f>
         <v>80.75</v>
       </c>
@@ -2157,25 +2151,25 @@
       <c r="B4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="50"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="50"/>
+      <c r="K5" s="53"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2195,10 +2189,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="52">
+      <c r="K6" s="57">
         <f>F7+F13+F20+F43+F45+F47+F46+J76</f>
         <v>31.5</v>
       </c>
@@ -2221,8 +2215,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="52"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2242,8 +2236,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="52"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2263,12 +2257,12 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="53" t="s">
+      <c r="J9" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="52">
+      <c r="K9" s="57">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74</f>
-        <v>75.260000000000005</v>
+        <v>79.27000000000001</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2288,8 +2282,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="57"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2306,8 +2300,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="52"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2326,10 +2320,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="52">
+      <c r="K12" s="57">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77</f>
         <v>36.6</v>
       </c>
@@ -2349,8 +2343,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="52"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="57"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2367,8 +2361,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="52"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="57"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2385,10 +2379,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="52">
+      <c r="K15" s="57">
         <f>F10+F16+F39+F40+F49+F50+F51+J75</f>
         <v>28</v>
       </c>
@@ -2408,8 +2402,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="52"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="57"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2426,8 +2420,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="52"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="57"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2446,10 +2440,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="56" t="s">
+      <c r="J18" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="52">
+      <c r="K18" s="57">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+F79+F82+F81+J78</f>
         <v>30.25</v>
       </c>
@@ -2472,8 +2466,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="52"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="57"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2492,8 +2486,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="52"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="57"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2530,11 +2524,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="57" t="s">
+      <c r="J22" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2859,19 +2853,19 @@
       <c r="B41" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="59"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3546,11 +3540,11 @@
       <c r="B72" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
+      <c r="C72" s="50"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="50"/>
+      <c r="G72" s="50"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3562,12 +3556,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="59"/>
-      <c r="C73" s="60"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="60"/>
-      <c r="F73" s="60"/>
-      <c r="G73" s="60"/>
+      <c r="B73" s="51"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="F73" s="52"/>
+      <c r="G73" s="52"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -3576,8 +3570,8 @@
         <v>31.55</v>
       </c>
       <c r="K73">
-        <f>E74+E83+E92+E93+E94+E95</f>
-        <v>11</v>
+        <f>E74+E83+E92+E93+E94+E95+E105+E106+E107+E108+E109+E110+E111+E122+E122+E122+E123</f>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3602,11 +3596,11 @@
       </c>
       <c r="J74">
         <f>F80+F91+F102+F104+F103+F118+F119+F120</f>
-        <v>29.54</v>
+        <v>33.549999999999997</v>
       </c>
       <c r="K74">
         <f>E80+E91+E102+E103+E104+E118+E119+E120</f>
-        <v>25.5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3651,12 +3645,12 @@
         <v>12</v>
       </c>
       <c r="J76">
-        <f>F75+F89+F90+F99+F100</f>
+        <f>F75+F89+F90+F99+F100+F115+F116+F117</f>
         <v>0</v>
       </c>
       <c r="K76">
-        <f>E75+E89+E90+E99+E100</f>
-        <v>3</v>
+        <f>E75+E89+E90+E99+E100+E115+E116+E117</f>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3680,7 +3674,7 @@
         <v>0</v>
       </c>
       <c r="K77">
-        <f>E84+E85+E86+E87</f>
+        <f>E84+E85+E86+E87+E112+E113+E114</f>
         <v>3</v>
       </c>
     </row>
@@ -3701,12 +3695,12 @@
         <v>16</v>
       </c>
       <c r="J78">
-        <f>F79+F81+F82+F97</f>
+        <f>F79+F81+F82+F97+F121</f>
         <v>7</v>
       </c>
       <c r="K78">
-        <f>E79+E82+E81</f>
-        <v>12</v>
+        <f>E79+E82+E81+E97+E121</f>
+        <v>12.5</v>
       </c>
     </row>
     <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4107,7 +4101,7 @@
         <v>2</v>
       </c>
       <c r="F103" s="1">
-        <v>4.17</v>
+        <v>4.34</v>
       </c>
       <c r="G103" s="11"/>
     </row>
@@ -4152,7 +4146,7 @@
         <v>9</v>
       </c>
       <c r="C106" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D106" s="34" t="s">
         <v>11</v>
@@ -4170,7 +4164,7 @@
         <v>9</v>
       </c>
       <c r="C107" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D107" s="34" t="s">
         <v>11</v>
@@ -4188,7 +4182,7 @@
         <v>9</v>
       </c>
       <c r="C108" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D108" s="34" t="s">
         <v>11</v>
@@ -4353,7 +4347,7 @@
         <v>5</v>
       </c>
       <c r="F118" s="34">
-        <v>7</v>
+        <v>10.84</v>
       </c>
       <c r="G118" s="11"/>
     </row>
@@ -4380,11 +4374,11 @@
         <v>13</v>
       </c>
       <c r="C120" s="46" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D120" s="46"/>
       <c r="E120" s="46">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F120" s="46">
         <v>1.5</v>
@@ -4404,7 +4398,7 @@
         <v>9</v>
       </c>
       <c r="C122" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D122" s="34" t="s">
         <v>11</v>
@@ -4422,7 +4416,7 @@
         <v>9</v>
       </c>
       <c r="C123" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D123" s="34" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
juego online, actualizacíon horas
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 3ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 3ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanzc\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E34721B-9485-4FFF-A2B3-8DEAB0AF5D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BB8567-6F06-4950-AB7B-1FEC9058AE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,7 @@
   <authors>
     <author>tc={9371C6CE-05AE-48D9-9CC4-7BBBBF016020}</author>
     <author>tc={779B0B16-BA1A-4FB6-BFB9-BA670422C61C}</author>
+    <author>tc={DCADFB7B-A4CD-4265-8258-B2317A485A47}</author>
   </authors>
   <commentList>
     <comment ref="C98" authorId="0" shapeId="0" xr:uid="{9371C6CE-05AE-48D9-9CC4-7BBBBF016020}">
@@ -59,12 +60,20 @@
      (Un comando para instalar y otro para arrancar)</t>
       </text>
     </comment>
+    <comment ref="C124" authorId="2" shapeId="0" xr:uid="{DCADFB7B-A4CD-4265-8258-B2317A485A47}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+     (Un comando para instalar y otro para arrancar)</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="174">
   <si>
     <t>Nombre</t>
   </si>
@@ -585,6 +594,9 @@
   </si>
   <si>
     <t>boton de volumen (mutear)</t>
+  </si>
+  <si>
+    <t>Arrancar la aplicación con render</t>
   </si>
 </sst>
 </file>
@@ -594,7 +606,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -667,6 +679,12 @@
       <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -2074,6 +2092,9 @@
   <threadedComment ref="C99" dT="2023-10-19T08:57:35.81" personId="{9E3B25B0-60DB-4849-A9FC-31D877943E05}" id="{779B0B16-BA1A-4FB6-BFB9-BA670422C61C}">
     <text xml:space="preserve"> (Un comando para instalar y otro para arrancar)</text>
   </threadedComment>
+  <threadedComment ref="C124" dT="2023-10-19T08:57:35.81" personId="{9E3B25B0-60DB-4849-A9FC-31D877943E05}" id="{DCADFB7B-A4CD-4265-8258-B2317A485A47}">
+    <text xml:space="preserve"> (Un comando para instalar y otro para arrancar)</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2082,25 +2103,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P123"/>
+  <dimension ref="A2:P124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="35.42578125" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.26953125" customWidth="1"/>
+    <col min="11" max="11" width="35.453125" customWidth="1"/>
+    <col min="12" max="12" width="26.7265625" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2126,7 +2147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2139,16 +2160,16 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>313.71999999999997</v>
+        <v>320.46999999999997</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
       <c r="K3" s="54">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73</f>
-        <v>80.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="50" t="s">
         <v>8</v>
       </c>
@@ -2162,7 +2183,7 @@
       </c>
       <c r="K4" s="54"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="52"/>
       <c r="C5" s="53"/>
       <c r="D5" s="53"/>
@@ -2175,7 +2196,7 @@
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2201,7 +2222,7 @@
       <c r="M6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -2222,7 +2243,7 @@
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
@@ -2243,7 +2264,7 @@
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
@@ -2268,7 +2289,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
@@ -2286,7 +2307,7 @@
       <c r="J10" s="60"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
@@ -2306,7 +2327,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
@@ -2329,7 +2350,7 @@
         <v>44.85</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
@@ -2347,7 +2368,7 @@
       <c r="J13" s="63"/>
       <c r="K13" s="58"/>
     </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2365,7 +2386,7 @@
       <c r="J14" s="64"/>
       <c r="K14" s="58"/>
     </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
@@ -2388,7 +2409,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
@@ -2406,7 +2427,7 @@
       <c r="J16" s="66"/>
       <c r="K16" s="58"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
@@ -2424,7 +2445,7 @@
       <c r="J17" s="67"/>
       <c r="K17" s="58"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>16</v>
       </c>
@@ -2449,7 +2470,7 @@
         <v>30.25</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2470,7 +2491,7 @@
       <c r="J19" s="69"/>
       <c r="K19" s="58"/>
     </row>
-    <row r="20" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2490,7 +2511,7 @@
       <c r="J20" s="69"/>
       <c r="K20" s="58"/>
     </row>
-    <row r="21" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2508,7 +2529,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2531,7 +2552,7 @@
       <c r="K22" s="70"/>
       <c r="L22" s="70"/>
     </row>
-    <row r="23" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2549,7 +2570,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2567,7 +2588,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2585,7 +2606,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2603,7 +2624,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2621,7 +2642,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2639,7 +2660,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2657,7 +2678,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2675,7 +2696,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2692,7 +2713,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2710,7 +2731,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2726,7 +2747,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2744,7 +2765,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2762,7 +2783,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2780,7 +2801,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2798,7 +2819,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2816,7 +2837,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2834,7 +2855,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2852,7 +2873,7 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B41" s="50" t="s">
         <v>36</v>
       </c>
@@ -2862,7 +2883,7 @@
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
     </row>
-    <row r="42" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B42" s="52"/>
       <c r="C42" s="53"/>
       <c r="D42" s="53"/>
@@ -2870,7 +2891,7 @@
       <c r="F42" s="53"/>
       <c r="G42" s="53"/>
     </row>
-    <row r="43" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -2888,7 +2909,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -2906,7 +2927,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -2924,7 +2945,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2942,7 +2963,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -2960,7 +2981,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -2978,7 +2999,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -3005,7 +3026,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -3034,7 +3055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -3063,7 +3084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -3092,7 +3113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -3121,7 +3142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -3150,7 +3171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -3177,7 +3198,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -3195,7 +3216,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -3213,7 +3234,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -3240,7 +3261,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -3269,7 +3290,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -3298,7 +3319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3325,7 +3346,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>9</v>
       </c>
@@ -3354,7 +3375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>9</v>
       </c>
@@ -3383,7 +3404,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>9</v>
       </c>
@@ -3412,7 +3433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
         <v>9</v>
       </c>
@@ -3430,7 +3451,7 @@
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
         <v>13</v>
       </c>
@@ -3449,7 +3470,7 @@
       </c>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>14</v>
       </c>
@@ -3467,7 +3488,7 @@
       </c>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>14</v>
       </c>
@@ -3485,7 +3506,7 @@
       </c>
       <c r="G68" s="26"/>
     </row>
-    <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
         <v>16</v>
       </c>
@@ -3503,7 +3524,7 @@
       </c>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
         <v>16</v>
       </c>
@@ -3521,7 +3542,7 @@
       </c>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>9</v>
       </c>
@@ -3539,7 +3560,7 @@
       </c>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="50" t="s">
         <v>67</v>
       </c>
@@ -3558,7 +3579,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="52"/>
       <c r="C73" s="53"/>
       <c r="D73" s="53"/>
@@ -3569,15 +3590,15 @@
         <v>9</v>
       </c>
       <c r="J73">
-        <f>F74+F83+F92+F93+F94+F95+F108+F109+F110+F111+F122+F123+F105+F106+F107</f>
-        <v>31.55</v>
+        <f>F74+F83+F92+F93+F94+F95+F108+F109+F110+F111+F122+F123+F105+F106+F107+F124</f>
+        <v>38.299999999999997</v>
       </c>
       <c r="K73">
-        <f>E74+E83+E92+E93+E94+E95+E105+E106+E107+E108+E109+E110+E111+E122+E122+E122+E123</f>
+        <f>E74+E83+E92+E93+E94+E95+E105+E106+E107+E108+E109+E110+E111+E122+E122+E122+E123+E124</f>
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
         <v>9</v>
       </c>
@@ -3606,7 +3627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>12</v>
       </c>
@@ -3635,7 +3656,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>15</v>
       </c>
@@ -3662,7 +3683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
         <v>15</v>
       </c>
@@ -3691,7 +3712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="9" t="s">
         <v>15</v>
       </c>
@@ -3720,7 +3741,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="s">
         <v>16</v>
       </c>
@@ -3736,7 +3757,7 @@
       </c>
       <c r="G79" s="11"/>
     </row>
-    <row r="80" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="s">
         <v>13</v>
       </c>
@@ -3752,7 +3773,7 @@
       </c>
       <c r="G80" s="11"/>
     </row>
-    <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
         <v>16</v>
       </c>
@@ -3766,7 +3787,7 @@
       <c r="F81" s="34"/>
       <c r="G81" s="34"/>
     </row>
-    <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="10" t="s">
         <v>16</v>
       </c>
@@ -3784,7 +3805,7 @@
       </c>
       <c r="G82" s="11"/>
     </row>
-    <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>9</v>
       </c>
@@ -3802,7 +3823,7 @@
       </c>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="s">
         <v>14</v>
       </c>
@@ -3816,7 +3837,7 @@
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -3830,7 +3851,7 @@
       <c r="F85" s="34"/>
       <c r="G85" s="34"/>
     </row>
-    <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>14</v>
       </c>
@@ -3844,7 +3865,7 @@
       <c r="F86" s="34"/>
       <c r="G86" s="34"/>
     </row>
-    <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="36" t="s">
         <v>14</v>
       </c>
@@ -3862,7 +3883,7 @@
       </c>
       <c r="G87" s="37"/>
     </row>
-    <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="9" t="s">
         <v>15</v>
       </c>
@@ -3880,7 +3901,7 @@
       </c>
       <c r="G88" s="49"/>
     </row>
-    <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
         <v>12</v>
       </c>
@@ -3898,7 +3919,7 @@
       </c>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>12</v>
       </c>
@@ -3916,7 +3937,7 @@
       </c>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
         <v>13</v>
       </c>
@@ -3934,7 +3955,7 @@
       </c>
       <c r="G91" s="11"/>
     </row>
-    <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
         <v>9</v>
       </c>
@@ -3952,7 +3973,7 @@
       </c>
       <c r="G92" s="11"/>
     </row>
-    <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>9</v>
       </c>
@@ -3970,7 +3991,7 @@
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="2:7" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:7" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -3988,7 +4009,7 @@
       </c>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
         <v>9</v>
       </c>
@@ -4006,7 +4027,7 @@
       </c>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="40" t="s">
         <v>15</v>
       </c>
@@ -4024,7 +4045,7 @@
       </c>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="10" t="s">
         <v>16</v>
       </c>
@@ -4042,7 +4063,7 @@
       </c>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="37" t="s">
         <v>150</v>
       </c>
@@ -4056,7 +4077,7 @@
       <c r="F98" s="37"/>
       <c r="G98" s="11"/>
     </row>
-    <row r="99" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>12</v>
       </c>
@@ -4074,7 +4095,7 @@
       </c>
       <c r="G99" s="11"/>
     </row>
-    <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>12</v>
       </c>
@@ -4090,7 +4111,7 @@
       </c>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="40" t="s">
         <v>15</v>
       </c>
@@ -4108,7 +4129,7 @@
       </c>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="6" t="s">
         <v>13</v>
       </c>
@@ -4124,7 +4145,7 @@
       </c>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
         <v>13</v>
       </c>
@@ -4142,7 +4163,7 @@
       </c>
       <c r="G103" s="11"/>
     </row>
-    <row r="104" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
         <v>13</v>
       </c>
@@ -4160,7 +4181,7 @@
       </c>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="42" t="s">
         <v>9</v>
       </c>
@@ -4178,7 +4199,7 @@
       </c>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="42" t="s">
         <v>9</v>
       </c>
@@ -4196,7 +4217,7 @@
       </c>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="42" t="s">
         <v>9</v>
       </c>
@@ -4214,7 +4235,7 @@
       </c>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="42" t="s">
         <v>9</v>
       </c>
@@ -4232,7 +4253,7 @@
       </c>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="42" t="s">
         <v>9</v>
       </c>
@@ -4245,10 +4266,12 @@
       <c r="E109" s="34">
         <v>15</v>
       </c>
-      <c r="F109" s="34"/>
-      <c r="G109" s="34"/>
-    </row>
-    <row r="110" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F109" s="34">
+        <v>6</v>
+      </c>
+      <c r="G109" s="11"/>
+    </row>
+    <row r="110" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="42" t="s">
         <v>9</v>
       </c>
@@ -4266,7 +4289,7 @@
       </c>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="42" t="s">
         <v>9</v>
       </c>
@@ -4284,7 +4307,7 @@
       </c>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="43" t="s">
         <v>14</v>
       </c>
@@ -4298,7 +4321,7 @@
       <c r="F112" s="34"/>
       <c r="G112" s="34"/>
     </row>
-    <row r="113" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="44" t="s">
         <v>14</v>
       </c>
@@ -4312,7 +4335,7 @@
       <c r="F113" s="34"/>
       <c r="G113" s="34"/>
     </row>
-    <row r="114" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="44" t="s">
         <v>14</v>
       </c>
@@ -4326,7 +4349,7 @@
       <c r="F114" s="34"/>
       <c r="G114" s="34"/>
     </row>
-    <row r="115" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
         <v>12</v>
       </c>
@@ -4344,7 +4367,7 @@
       </c>
       <c r="G115" s="11"/>
     </row>
-    <row r="116" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
         <v>12</v>
       </c>
@@ -4358,7 +4381,7 @@
       <c r="F116" s="34"/>
       <c r="G116" s="34"/>
     </row>
-    <row r="117" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
         <v>12</v>
       </c>
@@ -4372,7 +4395,7 @@
       <c r="F117" s="34"/>
       <c r="G117" s="34"/>
     </row>
-    <row r="118" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="45" t="s">
         <v>13</v>
       </c>
@@ -4390,7 +4413,7 @@
       </c>
       <c r="G118" s="11"/>
     </row>
-    <row r="119" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="45" t="s">
         <v>13</v>
       </c>
@@ -4408,7 +4431,7 @@
       </c>
       <c r="G119" s="11"/>
     </row>
-    <row r="120" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="45" t="s">
         <v>13</v>
       </c>
@@ -4424,7 +4447,7 @@
       </c>
       <c r="G120" s="11"/>
     </row>
-    <row r="121" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="10" t="s">
         <v>16</v>
       </c>
@@ -4432,7 +4455,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="4" t="s">
         <v>9</v>
       </c>
@@ -4450,7 +4473,7 @@
       </c>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
         <v>9</v>
       </c>
@@ -4465,6 +4488,24 @@
       </c>
       <c r="F123" s="34"/>
       <c r="G123" s="48"/>
+    </row>
+    <row r="124" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="D124" s="37">
+        <v>48</v>
+      </c>
+      <c r="E124" s="37">
+        <v>0</v>
+      </c>
+      <c r="F124" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="G124" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -4501,17 +4542,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>91</v>
       </c>
@@ -4541,7 +4582,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -4570,7 +4611,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -4591,7 +4632,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -4614,7 +4655,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -4629,7 +4670,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -4648,7 +4689,7 @@
       </c>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -4671,7 +4712,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -4686,7 +4727,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -4709,7 +4750,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -4724,7 +4765,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -4739,7 +4780,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -4754,7 +4795,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -4769,7 +4810,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -4784,7 +4825,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -4799,7 +4840,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -4814,7 +4855,7 @@
       <c r="F16" s="13"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -4829,7 +4870,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -4850,7 +4891,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -4871,7 +4912,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -4888,7 +4929,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -4909,7 +4950,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -4924,7 +4965,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -4939,7 +4980,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -4960,7 +5001,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -4975,7 +5016,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -4998,7 +5039,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -5013,7 +5054,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -5036,7 +5077,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -5051,7 +5092,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -5066,7 +5107,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -5089,7 +5130,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -5110,7 +5151,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -5131,7 +5172,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -5152,7 +5193,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -5167,7 +5208,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -5182,7 +5223,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -5205,7 +5246,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -5220,7 +5261,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -5235,7 +5276,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -5256,7 +5297,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -5279,7 +5320,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -5302,7 +5343,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -5325,7 +5366,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -5348,7 +5389,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -5369,7 +5410,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -5384,7 +5425,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -5405,7 +5446,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>47</v>
       </c>
@@ -5428,7 +5469,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="38">
         <v>48</v>
       </c>
@@ -5451,12 +5492,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5669,17 +5709,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5704,18 +5754,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>